<commit_message>
Explore with jupyter notebook.
</commit_message>
<xml_diff>
--- a/model_statistics.xlsx
+++ b/model_statistics.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Projects\Quant\Quant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell-pc\Quant\Quant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8D8284-EC94-4755-ACCD-898D0E287211}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{49CFF7C7-3179-462F-AF06-E8052044F227}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6108" xr2:uid="{0AC0E055-5388-486B-B3C3-0690848CE20F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6105" xr2:uid="{0AC0E055-5388-486B-B3C3-0690848CE20F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -790,11 +790,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -836,7 +836,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1200,309 +1200,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F8B7A-5696-407A-BE4B-C1C38C1030FB}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14"/>
+    <row r="20" spans="1:14"/>
+    <row r="21" spans="1:14"/>
+    <row r="22" spans="1:14"/>
+    <row r="23" spans="1:14"/>
+    <row r="24" spans="1:14"/>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N27" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N28" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
         <v>15</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N29" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N30" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N31" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="35" spans="1:14"/>
+    <row r="36" spans="1:14"/>
+    <row r="37" spans="1:14"/>
+    <row r="38" spans="1:14"/>
+    <row r="39" spans="1:14"/>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
         <v>21</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="N40" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
         <v>22</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="N41" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
         <v>23</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N42" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="43" spans="1:14">
+      <c r="A43" t="s">
         <v>24</v>
       </c>
-      <c r="N27" s="3" t="s">
+      <c r="N43" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
         <v>25</v>
       </c>
-      <c r="N28" s="3" t="s">
+      <c r="N44" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
         <v>26</v>
       </c>
-      <c r="N29" s="4" t="s">
+      <c r="N45" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="49" spans="1:14">
+      <c r="A49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="50" spans="1:14"/>
+    <row r="51" spans="1:14"/>
+    <row r="52" spans="1:14"/>
+    <row r="53" spans="1:14"/>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
         <v>37</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="N54" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="55" spans="1:14">
+      <c r="A55" t="s">
         <v>38</v>
       </c>
-      <c r="N39" s="3" t="s">
+      <c r="N55" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="56" spans="1:14">
+      <c r="A56" t="s">
         <v>39</v>
       </c>
-      <c r="N40" s="3" t="s">
+      <c r="N56" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="57" spans="1:14">
+      <c r="A57" t="s">
         <v>40</v>
       </c>
-      <c r="N41" s="3" t="s">
+      <c r="N57" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="58" spans="1:14">
+      <c r="A58" t="s">
         <v>41</v>
       </c>
-      <c r="N42" s="3" t="s">
+      <c r="N58" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="59" spans="1:14">
+      <c r="A59" t="s">
         <v>42</v>
       </c>
-      <c r="N43" s="4" t="s">
+      <c r="N59" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="60" spans="1:14">
+      <c r="A60" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="61" spans="1:14">
+      <c r="A61" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="62" spans="1:14">
+      <c r="A62" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="63" spans="1:14">
+      <c r="A63" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>48</v>
-      </c>
-      <c r="N52" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>49</v>
-      </c>
-      <c r="N53" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>50</v>
-      </c>
-      <c r="N54" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>51</v>
-      </c>
-      <c r="N55" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>52</v>
-      </c>
-      <c r="N56" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>53</v>
-      </c>
-      <c r="N57" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>57</v>
-      </c>
-    </row>
+    <row r="64" spans="1:14"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>